<commit_message>
fix : fix error due to poor connexion
</commit_message>
<xml_diff>
--- a/data-raw/variables.xlsx
+++ b/data-raw/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\SIVA\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE2EF8CF-B9BE-4983-B70F-67BC5EEA535D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1697A0B1-5842-4920-B2E5-AA10BC8A73F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="1" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="niveaux" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3379" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3476" uniqueCount="597">
   <si>
     <t>Tag</t>
   </si>
@@ -2912,14 +2912,1229 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ABF0A0-878B-4426-BEED-9AC76AA007A9}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1005</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2">
+        <v>16</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>1588</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3">
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1900</v>
+      </c>
+      <c r="B4">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>303</v>
+      </c>
+      <c r="J4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>1903</v>
+      </c>
+      <c r="B5">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>310</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="J5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>1904</v>
+      </c>
+      <c r="B6">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>311</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>78</v>
+      </c>
+      <c r="K6" t="s">
+        <v>72</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>1905</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>312</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>1</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A8">
+        <v>2515</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>325</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>303</v>
+      </c>
+      <c r="J8" t="s">
+        <v>151</v>
+      </c>
+      <c r="K8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8">
+        <v>3</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A9">
+        <v>2523</v>
+      </c>
+      <c r="B9">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>328</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>303</v>
+      </c>
+      <c r="J9" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" t="s">
+        <v>117</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>2</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A10">
+        <v>2536</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>338</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>339</v>
+      </c>
+      <c r="I10" t="s">
+        <v>340</v>
+      </c>
+      <c r="J10" t="s">
+        <v>341</v>
+      </c>
+      <c r="K10" t="s">
+        <v>134</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>2</v>
+      </c>
+      <c r="N10">
+        <v>2</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>1</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A11">
+        <v>2537</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>342</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>340</v>
+      </c>
+      <c r="J11" t="s">
+        <v>341</v>
+      </c>
+      <c r="K11" t="s">
+        <v>134</v>
+      </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>2</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A12">
+        <v>2538</v>
+      </c>
+      <c r="B12">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>343</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>340</v>
+      </c>
+      <c r="J12" t="s">
+        <v>341</v>
+      </c>
+      <c r="K12" t="s">
+        <v>134</v>
+      </c>
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+      <c r="N12">
+        <v>2</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>2539</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>340</v>
+      </c>
+      <c r="J13" t="s">
+        <v>341</v>
+      </c>
+      <c r="K13" t="s">
+        <v>134</v>
+      </c>
+      <c r="L13">
+        <v>3</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A14">
+        <v>2540</v>
+      </c>
+      <c r="B14">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>345</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>-2</v>
+      </c>
+      <c r="I14" t="s">
+        <v>340</v>
+      </c>
+      <c r="J14" t="s">
+        <v>341</v>
+      </c>
+      <c r="K14" t="s">
+        <v>134</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>1</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A15">
+        <v>2550</v>
+      </c>
+      <c r="B15">
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>346</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>340</v>
+      </c>
+      <c r="J15" t="s">
+        <v>341</v>
+      </c>
+      <c r="K15" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15">
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <v>2</v>
+      </c>
+      <c r="N15">
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A16">
+        <v>2551</v>
+      </c>
+      <c r="B16">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>347</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>340</v>
+      </c>
+      <c r="J16" t="s">
+        <v>341</v>
+      </c>
+      <c r="K16" t="s">
+        <v>134</v>
+      </c>
+      <c r="L16">
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <v>2</v>
+      </c>
+      <c r="N16">
+        <v>2</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A17">
+        <v>2552</v>
+      </c>
+      <c r="B17">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>348</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17" t="s">
+        <v>340</v>
+      </c>
+      <c r="J17" t="s">
+        <v>341</v>
+      </c>
+      <c r="K17" t="s">
+        <v>134</v>
+      </c>
+      <c r="L17">
+        <v>3</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A18">
+        <v>2553</v>
+      </c>
+      <c r="B18">
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>349</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>340</v>
+      </c>
+      <c r="J18" t="s">
+        <v>341</v>
+      </c>
+      <c r="K18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>2</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A19">
+        <v>2554</v>
+      </c>
+      <c r="B19">
+        <v>25</v>
+      </c>
+      <c r="C19" t="s">
+        <v>350</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>340</v>
+      </c>
+      <c r="J19" t="s">
+        <v>341</v>
+      </c>
+      <c r="K19" t="s">
+        <v>134</v>
+      </c>
+      <c r="L19">
+        <v>3</v>
+      </c>
+      <c r="M19">
+        <v>2</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A20">
+        <v>3000</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>352</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>303</v>
+      </c>
+      <c r="J20" t="s">
+        <v>353</v>
+      </c>
+      <c r="K20" t="s">
+        <v>354</v>
+      </c>
+      <c r="L20">
+        <v>7</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>2</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20">
+        <v>9</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A21">
+        <v>9560</v>
+      </c>
+      <c r="B21">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>151</v>
+      </c>
+      <c r="K21" t="s">
+        <v>117</v>
+      </c>
+      <c r="L21">
+        <v>16</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A22">
+        <v>30020</v>
+      </c>
+      <c r="B22">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>165</v>
+      </c>
+      <c r="K22" t="s">
+        <v>166</v>
+      </c>
+      <c r="L22">
+        <v>16</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2928,11 +4143,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3759C77C-4993-4FB9-8950-D5421D09C285}">
   <dimension ref="A1:R879"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:R879"/>
+    <sheetView topLeftCell="A852" workbookViewId="0">
+      <selection activeCell="A874" sqref="A874:XFD874"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="32.06640625" customWidth="1"/>
+    <col min="10" max="10" width="28.265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
partial fix pb volume siphon, vanne, passe #10
</commit_message>
<xml_diff>
--- a/data-raw/variables.xlsx
+++ b/data-raw/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\SIVA\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665A89E7-5155-4AE0-9750-1AA460F59099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5E776D-A641-4A6A-95B4-5E5469CAE566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1815" windowWidth="21600" windowHeight="10905" activeTab="3" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
   </bookViews>
@@ -3660,7 +3660,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3723,7 +3723,7 @@
         <v>709</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="F3" t="s">
         <v>62</v>
@@ -3743,7 +3743,7 @@
         <v>710</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>303</v>
       </c>
       <c r="F4" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
dev : version 0.1.1 check OK
</commit_message>
<xml_diff>
--- a/data-raw/variables.xlsx
+++ b/data-raw/variables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\SIVA\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5E776D-A641-4A6A-95B4-5E5469CAE566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A8C9A5-79AD-4A10-B3F8-E63B27F8DB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1800" yWindow="1815" windowWidth="21600" windowHeight="10905" activeTab="3" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
   </bookViews>
@@ -3660,11 +3660,12 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A7" sqref="A7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="27.33203125" customWidth="1"/>
     <col min="4" max="4" width="32.796875" customWidth="1"/>
     <col min="6" max="6" width="23.796875" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
dev : data change in variables
</commit_message>
<xml_diff>
--- a/data-raw/variables.xlsx
+++ b/data-raw/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\SIVA\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A8C9A5-79AD-4A10-B3F8-E63B27F8DB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1236517-1C77-4018-801A-660F0025F24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="1815" windowWidth="21600" windowHeight="10905" activeTab="3" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="20148" windowHeight="12000" activeTab="2" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="niveaux" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="713">
   <si>
     <t>Tag</t>
   </si>
@@ -2177,6 +2177,9 @@
   </si>
   <si>
     <t>ile_aux_pies_debit</t>
+  </si>
+  <si>
+    <t>guenrouet</t>
   </si>
 </sst>
 </file>
@@ -3231,8 +3234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB08D0E-26FC-4C0D-941D-AB587AB8D3DE}">
   <dimension ref="A1:N19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3287,7 +3290,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>614</v>
+        <v>712</v>
       </c>
       <c r="B3">
         <v>2000</v>
@@ -3659,8 +3662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ABF0A0-878B-4426-BEED-9AC76AA007A9}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:F7"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
dev : create variables for ISAC
</commit_message>
<xml_diff>
--- a/data-raw/variables.xlsx
+++ b/data-raw/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\SIVA\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1236517-1C77-4018-801A-660F0025F24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EF263E-54CC-45CA-ACBC-5A97E8A0B5DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="0" windowWidth="20148" windowHeight="12000" activeTab="2" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
+    <workbookView xWindow="450" yWindow="435" windowWidth="20145" windowHeight="12000" activeTab="2" xr2:uid="{8D1B9F0B-2403-48D1-89EA-A30FCAB91CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="niveaux" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3524" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3526" uniqueCount="715">
   <si>
     <t>Tag</t>
   </si>
@@ -2071,9 +2071,6 @@
     <t>isac_amont1</t>
   </si>
   <si>
-    <t>selected</t>
-  </si>
-  <si>
     <t>pluvio_barrage_10min</t>
   </si>
   <si>
@@ -2180,13 +2177,22 @@
   </si>
   <si>
     <t>guenrouet</t>
+  </si>
+  <si>
+    <t>isac</t>
+  </si>
+  <si>
+    <t>pluvio</t>
+  </si>
+  <si>
+    <t>tagstation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2204,6 +2210,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2229,10 +2241,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2539,7 +2552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2932,7 +2945,7 @@
         <v>29</v>
       </c>
       <c r="D19" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E19" t="s">
         <v>19</v>
@@ -2952,7 +2965,7 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
@@ -2992,7 +3005,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E22" t="s">
         <v>19</v>
@@ -3143,7 +3156,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B30">
         <v>3102</v>
@@ -3152,7 +3165,7 @@
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E30" t="s">
         <v>98</v>
@@ -3232,10 +3245,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB08D0E-26FC-4C0D-941D-AB587AB8D3DE}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3245,13 +3258,16 @@
     <col min="6" max="6" width="24.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>596</v>
       </c>
       <c r="B1" t="s">
         <v>660</v>
       </c>
+      <c r="C1" t="s">
+        <v>714</v>
+      </c>
       <c r="D1" t="s">
         <v>661</v>
       </c>
@@ -3262,10 +3278,13 @@
         <v>663</v>
       </c>
       <c r="G1" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
+        <v>712</v>
+      </c>
+      <c r="H1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>612</v>
       </c>
@@ -3284,13 +3303,16 @@
       <c r="F2" t="s">
         <v>76</v>
       </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B3">
         <v>2000</v>
@@ -3307,8 +3329,14 @@
       <c r="F3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>613</v>
       </c>
@@ -3327,8 +3355,14 @@
       <c r="F4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>597</v>
       </c>
@@ -3347,8 +3381,14 @@
       <c r="F5" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>616</v>
       </c>
@@ -3359,7 +3399,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E6" t="s">
         <v>19</v>
@@ -3367,8 +3407,14 @@
       <c r="F6" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>618</v>
       </c>
@@ -3379,7 +3425,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -3387,91 +3433,118 @@
       <c r="F7" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
+        <v>677</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2532</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>665</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>669</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>678</v>
       </c>
-      <c r="B8" s="2">
-        <v>2532</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B9" s="3">
+        <v>2533</v>
+      </c>
+      <c r="C9" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>665</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="D9" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>669</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>679</v>
       </c>
-      <c r="B9" s="2">
-        <v>2533</v>
-      </c>
-      <c r="C9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>680</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="B10" s="3">
         <v>2530</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="E10" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>668</v>
       </c>
-      <c r="G10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G10" s="3">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>677</v>
-      </c>
-      <c r="B11" s="2">
+        <v>676</v>
+      </c>
+      <c r="B11" s="3">
         <v>2531</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="F11" s="2" t="s">
+      <c r="E11" s="3" t="s">
+        <v>690</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>668</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G11" s="3">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>672</v>
       </c>
@@ -3484,14 +3557,20 @@
       <c r="D12" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F12" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>673</v>
       </c>
@@ -3504,21 +3583,24 @@
       <c r="D13" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
         <v>664</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>674</v>
       </c>
@@ -3531,21 +3613,24 @@
       <c r="D14" s="1" t="s">
         <v>649</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F14" t="s">
         <v>664</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>675</v>
       </c>
@@ -3558,23 +3643,26 @@
       <c r="D15" s="1" t="s">
         <v>650</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F15" t="s">
         <v>664</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B16" s="1">
         <v>380</v>
@@ -3583,18 +3671,24 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>687</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>692</v>
+        <v>686</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>691</v>
       </c>
       <c r="F16" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B17" s="1">
         <v>381</v>
@@ -3603,18 +3697,24 @@
         <v>3</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>692</v>
+        <v>687</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>691</v>
       </c>
       <c r="F17" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B18" s="1">
         <v>334</v>
@@ -3623,18 +3723,24 @@
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>685</v>
-      </c>
-      <c r="E18" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F18" t="s">
         <v>664</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B19" s="1">
         <v>358</v>
@@ -3643,13 +3749,19 @@
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="E19" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F19" t="s">
         <v>664</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3695,7 +3807,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B2">
         <v>3100</v>
@@ -3704,7 +3816,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E2" t="s">
         <v>303</v>
@@ -3715,7 +3827,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B3">
         <v>1528</v>
@@ -3724,7 +3836,7 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E3" t="s">
         <v>303</v>
@@ -3735,7 +3847,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B4">
         <v>1565</v>
@@ -3744,7 +3856,7 @@
         <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E4" t="s">
         <v>303</v>
@@ -3755,7 +3867,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B5">
         <v>1900</v>
@@ -3764,7 +3876,7 @@
         <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E5" t="s">
         <v>303</v>
@@ -3775,7 +3887,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B6">
         <v>2515</v>
@@ -3795,7 +3907,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B7">
         <v>2523</v>
@@ -3815,7 +3927,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B8">
         <v>3000</v>
@@ -3824,7 +3936,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E8" t="s">
         <v>303</v>
@@ -3835,13 +3947,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B9">
         <v>40001</v>
       </c>
       <c r="D9" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E9" t="s">
         <v>303</v>
@@ -3849,13 +3961,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B10">
         <v>40002</v>
       </c>
       <c r="D10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E10" t="s">
         <v>303</v>

</xml_diff>